<commit_message>
📝 Doc: Add test cases documents as xlsx and html formats
</commit_message>
<xml_diff>
--- a/docs/API-Test-Cases-NewsAPI.xlsx
+++ b/docs/API-Test-Cases-NewsAPI.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="239">
   <si>
     <t xml:space="preserve">Test Case ID</t>
   </si>
@@ -81,7 +81,7 @@
 - articles: non-empty array</t>
   </si>
   <si>
-    <t xml:space="preserve">Equivalence Partitioning</t>
+    <t xml:space="preserve">Smoke Testing</t>
   </si>
   <si>
     <t xml:space="preserve">AUTH_002</t>
@@ -92,6 +92,9 @@
   <si>
     <t xml:space="preserve">1. Set valid API key in Authorization header (with and without "Bearer" prefix).
 2. Send GET request to /everything endpoint with query parameter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equivalence Partitioning</t>
   </si>
   <si>
     <t xml:space="preserve">AUTH_003</t>
@@ -889,6 +892,95 @@
     <t xml:space="preserve">Verify API behavior with 'from' date exceeding 5 years limit.</t>
   </si>
   <si>
+    <t xml:space="preserve">- q: {variable}
+- from: date more than 5 years ago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Send GET request with from date older than 5 years.
+2. Verify error response.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRC_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify basic functionality of sources endpoint.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/top-headlines/sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Send GET request to sources endpoint.
+2. Verify response status code.
+3. Validate sources data structure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status: "ok"
+sources: array filled with news sources data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRC_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify sources filtering by valid category.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- category: All the valid values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Send GET request with category parameter.
+2. Verify response status code.
+3. Validate sources match selected category.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status: "ok"
+sources: array filtered by specified category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRC_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify sources filtering by valid language.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- language: All the valid values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Send GET request with language parameter.
+2. Verify response status code.
+3. Validate sources match selected language.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status: "ok"
+sources: array filtered by specified language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRC_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify sources filtering by valid country.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- country: All the valid values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Send GET request with country parameter.
+2. Verify response status code.
+3. Validate sources match selected language.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status: "ok"
+sources: array filtered by specified country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRC_005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify response with invalid category parameter.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -896,21 +988,127 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">- q: {variable}
-- </t>
+      <t xml:space="preserve">- category: ["invalid_category", "BUSINESS", "123", "!@#$%", "", null]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">from: date more than 5 years ago</t>
+      <t xml:space="preserve">Or other invalid values</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Send GET request with from date older than 5 years.
-2. Verify error response.</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Send GET request with invalid category.
+2. Verify successful response and make sure invalid params haven’t affected response.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status: "ok"
+sources: emptry array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRC_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify response with invalid language parameter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- language: ["invalid", "EN", "123", "!@#$%", "", null]
+(Or other invalid values)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Send GET request with invalid language.
+2. Verify successful response and make sure invalid params haven’t affected response.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status: “ok” 
+sources: emptry array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRC_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify response with invalid country parameter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- country: ["invalid_country", "US", "123", "!@#$%", "", null]
+(Or other invalid values)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Send GET request with invalid country.
+2. Verify successful response and make sure invalid params haven’t affected response.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THDL_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify successful basic request to /top-headlines endpoint.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/top-headlines</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- country: us </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Or any valid other country</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1010,12 +1208,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1035,17 +1233,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J48" activeCellId="0" sqref="J48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="84.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="75.72"/>
@@ -1148,15 +1346,15 @@
         <v>18</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>12</v>
@@ -1168,10 +1366,10 @@
         <v>14</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>17</v>
@@ -1180,15 +1378,15 @@
         <v>18</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>12</v>
@@ -1200,10 +1398,10 @@
         <v>14</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>17</v>
@@ -1212,15 +1410,15 @@
         <v>18</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>12</v>
@@ -1232,10 +1430,10 @@
         <v>14</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>17</v>
@@ -1244,15 +1442,15 @@
         <v>18</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>12</v>
@@ -1261,30 +1459,30 @@
         <v>13</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>12</v>
@@ -1293,30 +1491,30 @@
         <v>13</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>12</v>
@@ -1325,30 +1523,30 @@
         <v>13</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>12</v>
@@ -1360,27 +1558,27 @@
         <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>12</v>
@@ -1389,30 +1587,30 @@
         <v>13</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>12</v>
@@ -1421,19 +1619,19 @@
         <v>13</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J12" s="0" t="s">
         <v>19</v>
@@ -1441,10 +1639,10 @@
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>12</v>
@@ -1453,30 +1651,30 @@
         <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>12</v>
@@ -1485,30 +1683,30 @@
         <v>13</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>12</v>
@@ -1517,30 +1715,30 @@
         <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>12</v>
@@ -1549,30 +1747,30 @@
         <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>12</v>
@@ -1581,30 +1779,30 @@
         <v>13</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>12</v>
@@ -1613,30 +1811,30 @@
         <v>13</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>12</v>
@@ -1645,30 +1843,30 @@
         <v>13</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>12</v>
@@ -1677,30 +1875,30 @@
         <v>13</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>12</v>
@@ -1709,30 +1907,30 @@
         <v>13</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H21" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>12</v>
@@ -1741,30 +1939,30 @@
         <v>13</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>12</v>
@@ -1773,30 +1971,30 @@
         <v>13</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>12</v>
@@ -1805,30 +2003,30 @@
         <v>13</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>12</v>
@@ -1837,30 +2035,30 @@
         <v>13</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>12</v>
@@ -1869,62 +2067,62 @@
         <v>13</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="J27" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>12</v>
@@ -1933,30 +2131,30 @@
         <v>13</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>12</v>
@@ -1965,30 +2163,30 @@
         <v>13</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>12</v>
@@ -1997,30 +2195,30 @@
         <v>13</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>155</v>
+        <v>120</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>12</v>
@@ -2029,30 +2227,30 @@
         <v>13</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>160</v>
+        <v>120</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>12</v>
@@ -2061,30 +2259,30 @@
         <v>13</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H32" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>12</v>
@@ -2093,30 +2291,30 @@
         <v>13</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="G33" s="3" t="s">
         <v>169</v>
       </c>
+      <c r="G33" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="H33" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I33" s="3" t="s">
-        <v>170</v>
+      <c r="I33" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>12</v>
@@ -2125,30 +2323,30 @@
         <v>13</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G34" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="H34" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>165</v>
+      <c r="G34" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>12</v>
@@ -2157,30 +2355,30 @@
         <v>13</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="G35" s="3" t="s">
         <v>178</v>
       </c>
+      <c r="G35" s="2" t="s">
+        <v>179</v>
+      </c>
       <c r="H35" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I35" s="3" t="s">
-        <v>165</v>
+      <c r="I35" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>12</v>
@@ -2189,30 +2387,30 @@
         <v>13</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>183</v>
+        <v>120</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>12</v>
@@ -2221,62 +2419,62 @@
         <v>13</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H37" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>165</v>
+      <c r="I37" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B38" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="H38" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>165</v>
+      <c r="I38" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>12</v>
@@ -2285,30 +2483,30 @@
         <v>13</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="G39" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>194</v>
       </c>
+      <c r="G39" s="2" t="s">
+        <v>195</v>
+      </c>
       <c r="H39" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="I39" s="3" t="s">
-        <v>165</v>
+      <c r="I39" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>12</v>
@@ -2317,27 +2515,279 @@
         <v>13</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G40" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>68</v>
+      <c r="G40" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G41" s="3"/>
-      <c r="I41" s="3"/>
+      <c r="A41" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>